<commit_message>
removed old version, I will add new ones soon
</commit_message>
<xml_diff>
--- a/pre/illustrative table files/D-Link-IoT-Datasets.xlsx
+++ b/pre/illustrative table files/D-Link-IoT-Datasets.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahra\Desktop\GEMIDE\PCAPLAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e50b7f88a301451/Documents/GitHub/GEMIDE/pre/illustrative table files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7C098E1B-3A6A-4A53-83C9-7550F25147FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:40009_{7C098E1B-3A6A-4A53-83C9-7550F25147FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86A4EA9-7DA7-4F61-9698-10D65900162F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
   <si>
     <t>Dates</t>
   </si>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -564,7 +565,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -573,6 +574,11 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -632,9 +638,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -672,7 +678,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -778,7 +784,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -920,23 +926,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107:N127"/>
+    <sheetView topLeftCell="B108" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107:M127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -5200,41 +5211,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" ht="91.8" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>0</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G107" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H107" t="s">
+      <c r="H107" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J107" t="s">
+      <c r="J107" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K107" t="s">
+      <c r="K107" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="L107" t="s">
+      <c r="L107" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M107" t="s">
+      <c r="M107" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5362,84 +5373,84 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A111" s="2">
+      <c r="A111" s="8">
         <v>78</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="9">
         <v>44180</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C111" s="8">
         <v>3147</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111" s="8">
         <v>2103</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111" s="8">
         <v>3270</v>
       </c>
-      <c r="F111" s="2">
+      <c r="F111" s="8">
         <v>11776</v>
       </c>
-      <c r="G111" s="2">
+      <c r="G111" s="8">
         <v>70670</v>
       </c>
-      <c r="H111" s="2">
+      <c r="H111" s="8">
         <v>21958</v>
       </c>
-      <c r="I111" s="2">
+      <c r="I111" s="8">
         <v>21685</v>
       </c>
-      <c r="J111" s="2">
+      <c r="J111" s="8">
         <v>21899</v>
       </c>
-      <c r="K111" s="2">
-        <v>0</v>
-      </c>
-      <c r="L111" s="2">
+      <c r="K111" s="8">
+        <v>0</v>
+      </c>
+      <c r="L111" s="8">
         <v>21936</v>
       </c>
-      <c r="M111" s="2">
+      <c r="M111" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A112" s="2">
+      <c r="A112" s="8">
         <v>79</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="9">
         <v>44181</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C112" s="8">
         <v>2028</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112" s="8">
         <v>2114</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112" s="8">
         <v>2758</v>
       </c>
-      <c r="F112" s="2">
+      <c r="F112" s="8">
         <v>11425</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112" s="8">
         <v>69755</v>
       </c>
-      <c r="H112" s="2">
+      <c r="H112" s="8">
         <v>20721</v>
       </c>
-      <c r="I112" s="2">
+      <c r="I112" s="8">
         <v>20584</v>
       </c>
-      <c r="J112" s="2">
+      <c r="J112" s="8">
         <v>20743</v>
       </c>
-      <c r="K112" s="2">
-        <v>0</v>
-      </c>
-      <c r="L112" s="2">
+      <c r="K112" s="8">
+        <v>0</v>
+      </c>
+      <c r="L112" s="8">
         <v>9356</v>
       </c>
-      <c r="M112" s="2">
+      <c r="M112" s="8">
         <v>0</v>
       </c>
     </row>
@@ -6064,11 +6075,832 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB61C48-6F19-49E5-97DB-99EEE2EF2657}">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="A1:L21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="91.8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>44177</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5929</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5809</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5629</v>
+      </c>
+      <c r="E2" s="2">
+        <v>22163</v>
+      </c>
+      <c r="F2" s="2">
+        <v>32064</v>
+      </c>
+      <c r="G2" s="2">
+        <v>24986</v>
+      </c>
+      <c r="H2" s="2">
+        <v>24879</v>
+      </c>
+      <c r="I2" s="2">
+        <v>25111</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
+        <v>24848</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>44178</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3089</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2557</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3142</v>
+      </c>
+      <c r="E3" s="2">
+        <v>13841</v>
+      </c>
+      <c r="F3" s="2">
+        <v>72400</v>
+      </c>
+      <c r="G3" s="2">
+        <v>23017</v>
+      </c>
+      <c r="H3" s="2">
+        <v>22805</v>
+      </c>
+      <c r="I3" s="2">
+        <v>22968</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>22883</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44179</v>
+      </c>
+      <c r="B4">
+        <v>2760</v>
+      </c>
+      <c r="C4">
+        <v>2233</v>
+      </c>
+      <c r="D4">
+        <v>2533</v>
+      </c>
+      <c r="E4">
+        <v>18273</v>
+      </c>
+      <c r="F4">
+        <v>75237</v>
+      </c>
+      <c r="G4">
+        <v>26319</v>
+      </c>
+      <c r="H4">
+        <v>26340</v>
+      </c>
+      <c r="I4">
+        <v>27331</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>26141</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>44180</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3147</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2103</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3270</v>
+      </c>
+      <c r="E5" s="8">
+        <v>11776</v>
+      </c>
+      <c r="F5" s="8">
+        <v>70670</v>
+      </c>
+      <c r="G5" s="8">
+        <v>21958</v>
+      </c>
+      <c r="H5" s="8">
+        <v>21685</v>
+      </c>
+      <c r="I5" s="8">
+        <v>21899</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8">
+        <v>21936</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>44181</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2028</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2114</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2758</v>
+      </c>
+      <c r="E6" s="8">
+        <v>11425</v>
+      </c>
+      <c r="F6" s="8">
+        <v>69755</v>
+      </c>
+      <c r="G6" s="8">
+        <v>20721</v>
+      </c>
+      <c r="H6" s="8">
+        <v>20584</v>
+      </c>
+      <c r="I6" s="8">
+        <v>20743</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
+        <v>9356</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44182</v>
+      </c>
+      <c r="B7">
+        <v>728</v>
+      </c>
+      <c r="C7">
+        <v>932</v>
+      </c>
+      <c r="D7">
+        <v>919</v>
+      </c>
+      <c r="E7">
+        <v>11667</v>
+      </c>
+      <c r="F7">
+        <v>70001</v>
+      </c>
+      <c r="G7">
+        <v>19498</v>
+      </c>
+      <c r="H7">
+        <v>8221</v>
+      </c>
+      <c r="I7">
+        <v>20193</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>7222</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44184</v>
+      </c>
+      <c r="B8">
+        <v>1194</v>
+      </c>
+      <c r="C8">
+        <v>1326</v>
+      </c>
+      <c r="D8">
+        <v>1215</v>
+      </c>
+      <c r="E8">
+        <v>16964</v>
+      </c>
+      <c r="F8">
+        <v>42246</v>
+      </c>
+      <c r="G8">
+        <v>22604</v>
+      </c>
+      <c r="H8">
+        <v>15604</v>
+      </c>
+      <c r="I8">
+        <v>21296</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>9417</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>44185</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1839</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1839</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1916</v>
+      </c>
+      <c r="E9" s="2">
+        <v>28145</v>
+      </c>
+      <c r="F9" s="2">
+        <v>91359</v>
+      </c>
+      <c r="G9" s="2">
+        <v>24740</v>
+      </c>
+      <c r="H9" s="2">
+        <v>24638</v>
+      </c>
+      <c r="I9" s="2">
+        <v>24711</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>12607</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>44186</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1816</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1796</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1871</v>
+      </c>
+      <c r="E10" s="2">
+        <v>28669</v>
+      </c>
+      <c r="F10" s="2">
+        <v>90396</v>
+      </c>
+      <c r="G10" s="2">
+        <v>24566</v>
+      </c>
+      <c r="H10" s="2">
+        <v>24408</v>
+      </c>
+      <c r="I10" s="2">
+        <v>24571</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>12323</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44187</v>
+      </c>
+      <c r="B11">
+        <v>866</v>
+      </c>
+      <c r="C11">
+        <v>861</v>
+      </c>
+      <c r="D11">
+        <v>894</v>
+      </c>
+      <c r="E11">
+        <v>30515</v>
+      </c>
+      <c r="F11">
+        <v>88485</v>
+      </c>
+      <c r="G11">
+        <v>24026</v>
+      </c>
+      <c r="H11">
+        <v>11803</v>
+      </c>
+      <c r="I11">
+        <v>23918</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>11528</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>44195</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>31300</v>
+      </c>
+      <c r="F12">
+        <v>88834</v>
+      </c>
+      <c r="G12">
+        <v>25056</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>25063</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>10921</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>44196</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>28939</v>
+      </c>
+      <c r="F13">
+        <v>86678</v>
+      </c>
+      <c r="G13">
+        <v>23028</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>23005</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>10939</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>44197</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>29090</v>
+      </c>
+      <c r="F14">
+        <v>86837</v>
+      </c>
+      <c r="G14">
+        <v>23082</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>23011</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>10965</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44198</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>29391</v>
+      </c>
+      <c r="F15">
+        <v>86953</v>
+      </c>
+      <c r="G15">
+        <v>23094</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>23049</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>11070</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>44199</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>29298</v>
+      </c>
+      <c r="F16">
+        <v>86603</v>
+      </c>
+      <c r="G16">
+        <v>23054</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>22974</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>10953</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44202</v>
+      </c>
+      <c r="B17">
+        <v>970</v>
+      </c>
+      <c r="C17">
+        <v>993</v>
+      </c>
+      <c r="D17">
+        <v>1056</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44203</v>
+      </c>
+      <c r="B18">
+        <v>1874</v>
+      </c>
+      <c r="C18">
+        <v>1880</v>
+      </c>
+      <c r="D18">
+        <v>1829</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>44204</v>
+      </c>
+      <c r="B19">
+        <v>1829</v>
+      </c>
+      <c r="C19">
+        <v>1843</v>
+      </c>
+      <c r="D19">
+        <v>1971</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>44205</v>
+      </c>
+      <c r="B20">
+        <v>1423</v>
+      </c>
+      <c r="C20">
+        <v>1438</v>
+      </c>
+      <c r="D20">
+        <v>1501</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>44206</v>
+      </c>
+      <c r="B21">
+        <v>543</v>
+      </c>
+      <c r="C21">
+        <v>505</v>
+      </c>
+      <c r="D21">
+        <v>436</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>